<commit_message>
Add calc of 2020 ART/VMMC to Excel sheet
</commit_message>
<xml_diff>
--- a/Config/ART_coverage_data.xlsx
+++ b/Config/ART_coverage_data.xlsx
@@ -1,51 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E3BAF7-3604-4B42-AFFA-73F674C16D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empirical data" sheetId="6" r:id="rId1"/>
     <sheet name="Plots and estimates" sheetId="7" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Plots and estimates'!$B$35:$B$49</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Plots and estimates'!$C$35:$C$49</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Plots and estimates'!$C$35:$C$49</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Plots and estimates'!$D$35:$D$49</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Plots and estimates'!$D$35:$D$49</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Plots and estimates'!$B$35:$B$49</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Plots and estimates'!$C$35:$C$49</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Plots and estimates'!$D$35:$D$49</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Plots and estimates'!$B$35:$B$49</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Plots and estimates'!$C$35:$C$49</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Plots and estimates'!$D$35:$D$49</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Plots and estimates'!$B$35:$B$49</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="104">
   <si>
     <t>Source</t>
   </si>
@@ -365,16 +346,23 @@
   <si>
     <t>Empirical data</t>
   </si>
+  <si>
+    <t>interim calculation assuming linear scale-up to 90-90-90 by 2030</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000000000%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +401,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -435,12 +430,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -448,11 +443,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -468,11 +478,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +550,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1199,7 +1218,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1231,7 +1249,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1239,6 +1256,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1321,7 +1339,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2128,7 +2145,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2160,7 +2176,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2168,6 +2183,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3653,7 +3669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5042,11 +5058,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5054,8 +5070,8 @@
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="10" width="18.42578125" customWidth="1"/>
@@ -6034,394 +6050,545 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="17">
         <v>2004</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="17">
         <v>0</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="17">
         <v>0</v>
       </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="17">
         <v>2005</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="17">
         <f t="shared" ref="C36:C42" si="0">((G4*0.7)/(0.74 + 0.26*0.63))</f>
         <v>7.7450763443239652E-3</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="17">
         <f>0.74*C36</f>
         <v>5.7313564947997341E-3</v>
       </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="17">
         <v>2006</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="17">
         <f t="shared" si="0"/>
         <v>2.9431290108431069E-2</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="17">
         <f>0.74*C37</f>
         <v>2.1779154680238992E-2</v>
       </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="17">
         <v>2007</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="17">
         <f t="shared" si="0"/>
         <v>6.4284133657888917E-2</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="17">
         <f t="shared" ref="D38:D42" si="1">0.74*C38</f>
         <v>4.7570258906837797E-2</v>
       </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="17">
         <v>2008</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="17">
         <f t="shared" si="0"/>
         <v>0.11075459172383269</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="17">
         <f t="shared" si="1"/>
         <v>8.1958397875636191E-2</v>
       </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="17">
         <v>2009</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="17">
         <f t="shared" si="0"/>
         <v>0.15567603452091172</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="17">
         <f t="shared" si="1"/>
         <v>0.11520026554547468</v>
       </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="17">
         <v>2010</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="17">
         <f t="shared" si="0"/>
         <v>0.19130338570480196</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="17">
         <f t="shared" si="1"/>
         <v>0.14156450542155344</v>
       </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="13">
+      <c r="B42" s="17">
         <v>2011</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="17">
         <f t="shared" si="0"/>
         <v>0.23777384377074573</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D42" s="17">
         <f t="shared" si="1"/>
         <v>0.17595264439035183</v>
       </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="17">
         <v>2012</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43">
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18">
         <f>J13</f>
         <v>0.36000000000000004</v>
       </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="17">
         <v>2013</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B45" s="17">
         <v>2014</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="17">
         <v>2015</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="F46" s="1">
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19">
         <f>J14</f>
         <v>0.39900000000000002</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="19">
         <f>J16</f>
         <v>0.308</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="13">
+      <c r="B47" s="17">
         <v>2016</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="F47" s="1">
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="19">
         <f>J15</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="19">
         <f>J17</f>
         <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="13">
+      <c r="B48" s="17">
         <v>2017</v>
       </c>
-      <c r="C48" s="13">
+      <c r="C48" s="17">
         <f>((J11*0.8)/(0.74 + 0.26*0.63))</f>
         <v>0.59747731799070602</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="17">
         <f t="shared" ref="D48" si="2">0.74*C48</f>
         <v>0.44213321531312244</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="18">
         <f>J11*0.85</f>
         <v>0.57374999999999998</v>
       </c>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="13">
+      <c r="B49" s="20">
         <v>2018</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="20">
         <v>2004</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="18">
         <v>2005</v>
       </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="18">
         <v>2006</v>
       </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="18">
         <v>2007</v>
       </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="18">
         <v>2008</v>
       </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="18">
         <v>2009</v>
       </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="18">
         <v>2010</v>
       </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="18">
         <v>2011</v>
       </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="18">
         <v>2012</v>
       </c>
-      <c r="E58" s="1">
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19">
         <f>J28</f>
         <v>0.23799999999999999</v>
       </c>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="18">
         <v>2013</v>
       </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="18">
         <v>2014</v>
       </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="18">
         <v>2015</v>
       </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="18">
         <v>2016</v>
       </c>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="18">
         <v>2017</v>
       </c>
-      <c r="E63" s="1">
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="19">
         <f>J30</f>
         <v>0.52446974999999996</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="19">
         <f>J20</f>
         <v>0.57703034200000003</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="19">
         <f>J23</f>
         <v>0.43161612000000005</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="18">
         <v>2018</v>
       </c>
-      <c r="E64" s="1">
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19">
         <f>J29</f>
         <v>0.54</v>
+      </c>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="13">
+        <v>2020</v>
+      </c>
+      <c r="C66" s="21">
+        <f>C48+($B66-$B48)*H68</f>
+        <v>0.62782870614669695</v>
+      </c>
+      <c r="D66" s="21">
+        <f>D48+($B66-$B48)*I68</f>
+        <v>0.50833324254855572</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H67" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="13">
+        <v>2030</v>
+      </c>
+      <c r="C68" s="13">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="D68" s="13">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13">
+        <f>(C68-C48)/(($B68-1)-($B48-1))</f>
+        <v>1.0117129385330305E-2</v>
+      </c>
+      <c r="I68" s="13">
+        <f>(D68-D48)/(($B68-1)-($B48-1))</f>
+        <v>2.2066675745144426E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6431,6 +6598,9 @@
     <sortCondition ref="D4:D30"/>
     <sortCondition ref="F4:F30"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="H67:I67"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Add 2021 ART+VScov assuming 2017-2030 scale-up
</commit_message>
<xml_diff>
--- a/Config/ART_coverage_data.xlsx
+++ b/Config/ART_coverage_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E3BAF7-3604-4B42-AFFA-73F674C16D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DD69BD-4030-4E1A-9504-F0C53BC9FB09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empirical data" sheetId="6" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000000000%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -479,9 +479,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -492,7 +489,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5062,7 +5062,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6050,512 +6050,512 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>2004</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="16">
         <v>0</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="16">
         <v>0</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>2005</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="16">
         <f t="shared" ref="C36:C42" si="0">((G4*0.7)/(0.74 + 0.26*0.63))</f>
         <v>7.7450763443239652E-3</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="16">
         <f>0.74*C36</f>
         <v>5.7313564947997341E-3</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>2006</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="16">
         <f t="shared" si="0"/>
         <v>2.9431290108431069E-2</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="16">
         <f>0.74*C37</f>
         <v>2.1779154680238992E-2</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>2007</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="16">
         <f t="shared" si="0"/>
         <v>6.4284133657888917E-2</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="16">
         <f t="shared" ref="D38:D42" si="1">0.74*C38</f>
         <v>4.7570258906837797E-2</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>2008</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="16">
         <f t="shared" si="0"/>
         <v>0.11075459172383269</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="16">
         <f t="shared" si="1"/>
         <v>8.1958397875636191E-2</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>2009</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="16">
         <f t="shared" si="0"/>
         <v>0.15567603452091172</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="16">
         <f t="shared" si="1"/>
         <v>0.11520026554547468</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>2010</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="16">
         <f t="shared" si="0"/>
         <v>0.19130338570480196</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="16">
         <f t="shared" si="1"/>
         <v>0.14156450542155344</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="16">
         <v>2011</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="16">
         <f t="shared" si="0"/>
         <v>0.23777384377074573</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="16">
         <f t="shared" si="1"/>
         <v>0.17595264439035183</v>
       </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>2012</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="18">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17">
         <f>J13</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <v>2013</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="16">
         <v>2014</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="16">
         <v>2015</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19">
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18">
         <f>J14</f>
         <v>0.39900000000000002</v>
       </c>
-      <c r="G46" s="19">
+      <c r="G46" s="18">
         <f>J16</f>
         <v>0.308</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="17">
+      <c r="B47" s="16">
         <v>2016</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="19">
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="18">
         <f>J15</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="G47" s="19">
+      <c r="G47" s="18">
         <f>J17</f>
         <v>0.42599999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B48" s="16">
         <v>2017</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="16">
         <f>((J11*0.8)/(0.74 + 0.26*0.63))</f>
         <v>0.59747731799070602</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="16">
         <f t="shared" ref="D48" si="2">0.74*C48</f>
         <v>0.44213321531312244</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="17">
         <f>J11*0.85</f>
         <v>0.57374999999999998</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B49" s="19">
         <v>2018</v>
       </c>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="19">
         <v>2004</v>
       </c>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="18">
+      <c r="B51" s="17">
         <v>2005</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="17">
         <v>2006</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B53" s="17">
         <v>2007</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="18">
+      <c r="B54" s="17">
         <v>2008</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B55" s="17">
         <v>2009</v>
       </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B56" s="17">
         <v>2010</v>
       </c>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="17">
         <v>2011</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B58" s="17">
         <v>2012</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="19">
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="18">
         <f>J28</f>
         <v>0.23799999999999999</v>
       </c>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="18">
+      <c r="B59" s="17">
         <v>2013</v>
       </c>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="18">
+      <c r="B60" s="17">
         <v>2014</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="17">
         <v>2015</v>
       </c>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="18"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="18">
+      <c r="B62" s="17">
         <v>2016</v>
       </c>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="18">
+      <c r="B63" s="17">
         <v>2017</v>
       </c>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="19">
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18">
         <f>J30</f>
         <v>0.52446974999999996</v>
       </c>
-      <c r="F63" s="19">
+      <c r="F63" s="18">
         <f>J20</f>
         <v>0.57703034200000003</v>
       </c>
-      <c r="G63" s="19">
+      <c r="G63" s="18">
         <f>J23</f>
         <v>0.43161612000000005</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="18">
+      <c r="B64" s="17">
         <v>2018</v>
       </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="19">
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18">
         <f>J29</f>
         <v>0.54</v>
       </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="13">
         <v>2020</v>
       </c>
-      <c r="C66" s="21">
+      <c r="C66" s="20">
         <f>C48+($B66-$B48)*H68</f>
         <v>0.62782870614669695</v>
       </c>
-      <c r="D66" s="21">
+      <c r="D66" s="20">
         <f>D48+($B66-$B48)*I68</f>
         <v>0.50833324254855572</v>
       </c>
@@ -6564,10 +6564,21 @@
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H67" s="14" t="s">
+      <c r="B67" s="13">
+        <v>2021</v>
+      </c>
+      <c r="C67" s="20">
+        <f>C48+($B67-$B48)*H68</f>
+        <v>0.63794583553202722</v>
+      </c>
+      <c r="D67" s="20">
+        <f>D48+($B67-$B48)*I68</f>
+        <v>0.53039991829370015</v>
+      </c>
+      <c r="H67" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="I67" s="14"/>
+      <c r="I67" s="21"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="13">

</xml_diff>